<commit_message>
try to use white kernel to fit the noise
</commit_message>
<xml_diff>
--- a/rastrigin/add_noise/loss_in_trail.xlsx
+++ b/rastrigin/add_noise/loss_in_trail.xlsx
@@ -1,15 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25601"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoe-my.sharepoint.com/personal/s1893474_ed_ac_uk/Documents/UG3/论文创作/git_of_project/Bayesian_Optimisation_PI_EI/rastrigin/add_noise/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="6" documentId="11_8968858156AF68DE2FFC9890E22D62B150BEC313" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F37E1F6C-80C8-4A4A-8C07-AFC98FD9B247}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-25950" yWindow="2160" windowWidth="24670" windowHeight="15480" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -31,12 +50,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -44,8 +63,15 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="宋体"/>
       <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <name val="宋体"/>
+      <family val="3"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -95,6 +121,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -141,7 +175,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -173,9 +207,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -207,6 +259,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -382,14 +452,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:E11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:E34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C32" sqref="C32"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -403,177 +475,555 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2">
-        <v>3.369576086223087</v>
+        <v>-0.18590714398727931</v>
       </c>
       <c r="C2">
-        <v>0.4193569258587979</v>
+        <v>4.7345739850166906</v>
       </c>
       <c r="D2">
-        <v>3.93890887323326</v>
+        <v>-27.860520705940399</v>
       </c>
       <c r="E2">
-        <v>4.153214599412988</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5">
+        <v>-11.28232661241171</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>4.87287039006022</v>
+        <v>3.904474567048418</v>
       </c>
       <c r="C3">
-        <v>1.37430527049047</v>
+        <v>-5.3611820179035412</v>
       </c>
       <c r="D3">
-        <v>3.510186993263042</v>
+        <v>0.84143148051810179</v>
       </c>
       <c r="E3">
-        <v>0.7839513006289579</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5">
+        <v>-14.658935858535621</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
       <c r="B4">
-        <v>4.41725646718578</v>
+        <v>-9.4354238735160081</v>
       </c>
       <c r="C4">
-        <v>2.825572281551668</v>
+        <v>6.9869524618864656</v>
       </c>
       <c r="D4">
-        <v>-0.5241423303155974</v>
+        <v>-2.8423754902753142</v>
       </c>
       <c r="E4">
-        <v>5.446251755709323</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5">
+        <v>-13.086113611252211</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
       <c r="B5">
-        <v>3.256186716824376</v>
+        <v>13.24249364910002</v>
       </c>
       <c r="C5">
-        <v>-0.7040219622498176</v>
+        <v>-15.58943633359875</v>
       </c>
       <c r="D5">
-        <v>4.013696957252043</v>
+        <v>-16.896981881477291</v>
       </c>
       <c r="E5">
-        <v>-0.4794392243950136</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>-18.78737594842103</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
       <c r="B6">
-        <v>3.270137670665404</v>
+        <v>-10.54266870855621</v>
       </c>
       <c r="C6">
-        <v>1.173625318837303</v>
+        <v>2.9360199803284961</v>
       </c>
       <c r="D6">
-        <v>3.257619183619563</v>
+        <v>-0.60473757443298659</v>
       </c>
       <c r="E6">
-        <v>4.496617060221455</v>
-      </c>
-    </row>
-    <row r="7" spans="1:5">
+        <v>-20.40659107084538</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
       <c r="B7">
-        <v>3.504866426086378</v>
+        <v>-16.69234557840511</v>
       </c>
       <c r="C7">
-        <v>1.299505924731594</v>
+        <v>-12.092139398640439</v>
       </c>
       <c r="D7">
-        <v>4.685491089518941</v>
+        <v>-13.903789982513331</v>
       </c>
       <c r="E7">
-        <v>0.5240629483564156</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5">
+        <v>-8.7251923540605567</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
       <c r="B8">
-        <v>3.429328338880793</v>
+        <v>13.509272060560001</v>
       </c>
       <c r="C8">
-        <v>5.03080616568021</v>
+        <v>0.1240192760302499</v>
       </c>
       <c r="D8">
-        <v>2.440707555497881</v>
+        <v>-15.39218934091809</v>
       </c>
       <c r="E8">
-        <v>-0.301153649300101</v>
-      </c>
-    </row>
-    <row r="9" spans="1:5">
+        <v>-9.3403207682897751</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
       <c r="B9">
-        <v>3.409916667672316</v>
+        <v>11.906047702626591</v>
       </c>
       <c r="C9">
-        <v>-0.4768256227551988</v>
+        <v>-0.94520274854371955</v>
       </c>
       <c r="D9">
-        <v>4.236442010813775</v>
+        <v>-20.58939296012095</v>
       </c>
       <c r="E9">
-        <v>2.00119661387143</v>
-      </c>
-    </row>
-    <row r="10" spans="1:5">
+        <v>6.9049908092847758</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
       <c r="B10">
-        <v>3.993213676066326</v>
+        <v>8.3355278205754804</v>
       </c>
       <c r="C10">
-        <v>3.472636343412026</v>
+        <v>-2.818541223937391</v>
       </c>
       <c r="D10">
-        <v>3.310483226393752</v>
+        <v>-20.478995031569639</v>
       </c>
       <c r="E10">
-        <v>0.06465618389460448</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5">
+        <v>-12.18979906910322</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
       <c r="B11">
-        <v>1.255225555060386</v>
+        <v>-10.575083333649021</v>
       </c>
       <c r="C11">
-        <v>1.216718680864046</v>
+        <v>4.0636270632259759</v>
       </c>
       <c r="D11">
-        <v>-0.03609204268503641</v>
+        <v>-3.5248200604716828</v>
       </c>
       <c r="E11">
-        <v>0.856689003115519</v>
+        <v>-15.98669583667956</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A12" s="1">
+        <v>10</v>
+      </c>
+      <c r="B12">
+        <v>-6.0494684369196694</v>
+      </c>
+      <c r="C12">
+        <v>-3.91714014206871</v>
+      </c>
+      <c r="D12">
+        <v>6.3588209661023853E-2</v>
+      </c>
+      <c r="E12">
+        <v>-21.850064525123411</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A13" s="1">
+        <v>11</v>
+      </c>
+      <c r="B13">
+        <v>1.186747949563459</v>
+      </c>
+      <c r="C13">
+        <v>-7.5214040060318048</v>
+      </c>
+      <c r="D13">
+        <v>-8.9226521987619023</v>
+      </c>
+      <c r="E13">
+        <v>-8.6107778235453161</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A14" s="1">
+        <v>12</v>
+      </c>
+      <c r="B14">
+        <v>-12.38347539048049</v>
+      </c>
+      <c r="C14">
+        <v>8.1488633576145695</v>
+      </c>
+      <c r="D14">
+        <v>-0.39369460730790168</v>
+      </c>
+      <c r="E14">
+        <v>-6.433170823041479</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A15" s="1">
+        <v>13</v>
+      </c>
+      <c r="B15">
+        <v>3.966024859741502</v>
+      </c>
+      <c r="C15">
+        <v>-6.3124577564464701</v>
+      </c>
+      <c r="D15">
+        <v>-1.601732817379506</v>
+      </c>
+      <c r="E15">
+        <v>-3.3072697574973451</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A16" s="1">
+        <v>14</v>
+      </c>
+      <c r="B16">
+        <v>-4.9456625296242791</v>
+      </c>
+      <c r="C16">
+        <v>3.460714092773951</v>
+      </c>
+      <c r="D16">
+        <v>-17.9977142783045</v>
+      </c>
+      <c r="E16">
+        <v>-12.312130600359779</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A17" s="1">
+        <v>15</v>
+      </c>
+      <c r="B17">
+        <v>-19.892475153908482</v>
+      </c>
+      <c r="C17">
+        <v>6.2771579198783876</v>
+      </c>
+      <c r="D17">
+        <v>-2.165590934708888</v>
+      </c>
+      <c r="E17">
+        <v>7.0430313100840776</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A18" s="1">
+        <v>16</v>
+      </c>
+      <c r="B18">
+        <v>-10.53484331940985</v>
+      </c>
+      <c r="C18">
+        <v>-11.648831422805181</v>
+      </c>
+      <c r="D18">
+        <v>-3.116176941599246</v>
+      </c>
+      <c r="E18">
+        <v>-12.54732559485787</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A19" s="1">
+        <v>17</v>
+      </c>
+      <c r="B19">
+        <v>-11.13552355801459</v>
+      </c>
+      <c r="C19">
+        <v>-18.038970812841129</v>
+      </c>
+      <c r="D19">
+        <v>-18.183065225328662</v>
+      </c>
+      <c r="E19">
+        <v>-16.420964988173949</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A20" s="1">
+        <v>18</v>
+      </c>
+      <c r="B20">
+        <v>-9.6297946027485501</v>
+      </c>
+      <c r="C20">
+        <v>-7.0856886493739406</v>
+      </c>
+      <c r="D20">
+        <v>-5.8665190649933088</v>
+      </c>
+      <c r="E20">
+        <v>-9.4191492370937731</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A21" s="1">
+        <v>19</v>
+      </c>
+      <c r="B21">
+        <v>0.15913414893274511</v>
+      </c>
+      <c r="C21">
+        <v>-7.7037227653942573</v>
+      </c>
+      <c r="D21">
+        <v>7.8063301654485819</v>
+      </c>
+      <c r="E21">
+        <v>-19.52491066706456</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A22" s="1">
+        <v>20</v>
+      </c>
+      <c r="B22">
+        <v>2.9711851955364028</v>
+      </c>
+      <c r="C22">
+        <v>-1.631760909435704</v>
+      </c>
+      <c r="D22">
+        <v>-7.5640481383582827</v>
+      </c>
+      <c r="E22">
+        <v>-0.63117922831116147</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A23" s="1">
+        <v>21</v>
+      </c>
+      <c r="B23">
+        <v>-0.92736043759418152</v>
+      </c>
+      <c r="C23">
+        <v>-5.2788101563880598</v>
+      </c>
+      <c r="D23">
+        <v>-7.4070582926205084</v>
+      </c>
+      <c r="E23">
+        <v>-2.7825529772540101</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A24" s="1">
+        <v>22</v>
+      </c>
+      <c r="B24">
+        <v>-17.710122407879489</v>
+      </c>
+      <c r="C24">
+        <v>-23.623422100159509</v>
+      </c>
+      <c r="D24">
+        <v>2.7989312744949468</v>
+      </c>
+      <c r="E24">
+        <v>-6.3434650434527242</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A25" s="1">
+        <v>23</v>
+      </c>
+      <c r="B25">
+        <v>-8.9092282022671476</v>
+      </c>
+      <c r="C25">
+        <v>0.37199798317105431</v>
+      </c>
+      <c r="D25">
+        <v>-12.42025793278215</v>
+      </c>
+      <c r="E25">
+        <v>-6.396043523581957</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A26" s="1">
+        <v>24</v>
+      </c>
+      <c r="B26">
+        <v>8.0152277586762466</v>
+      </c>
+      <c r="C26">
+        <v>-2.3064152717289592</v>
+      </c>
+      <c r="D26">
+        <v>-3.5513578482309138</v>
+      </c>
+      <c r="E26">
+        <v>11.401863026741561</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A27" s="1">
+        <v>25</v>
+      </c>
+      <c r="B27">
+        <v>-5.0782991429399154</v>
+      </c>
+      <c r="C27">
+        <v>-12.089012798107371</v>
+      </c>
+      <c r="D27">
+        <v>-10.00998443277923</v>
+      </c>
+      <c r="E27">
+        <v>-3.691166704786264</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A28" s="1">
+        <v>26</v>
+      </c>
+      <c r="B28">
+        <v>2.6593941583833431</v>
+      </c>
+      <c r="C28">
+        <v>3.3048633056485879</v>
+      </c>
+      <c r="D28">
+        <v>-7.9214743955867863</v>
+      </c>
+      <c r="E28">
+        <v>-14.87435682055145</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A29" s="1">
+        <v>27</v>
+      </c>
+      <c r="B29">
+        <v>-9.6342955150317895</v>
+      </c>
+      <c r="C29">
+        <v>-19.073154356345569</v>
+      </c>
+      <c r="D29">
+        <v>-6.5628455218262216</v>
+      </c>
+      <c r="E29">
+        <v>-10.127249388649821</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A30" s="1">
+        <v>28</v>
+      </c>
+      <c r="B30">
+        <v>0.56646624585179239</v>
+      </c>
+      <c r="C30">
+        <v>-2.1644289463456872</v>
+      </c>
+      <c r="D30">
+        <v>-1.7096109653375251</v>
+      </c>
+      <c r="E30">
+        <v>-11.59805682831894</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A31" s="1">
+        <v>29</v>
+      </c>
+      <c r="B31">
+        <v>-6.4438928666206188</v>
+      </c>
+      <c r="C31">
+        <v>-13.33288378213479</v>
+      </c>
+      <c r="D31">
+        <v>8.2007002233289246</v>
+      </c>
+      <c r="E31">
+        <v>-18.59569993642776</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B33">
+        <f>AVERAGE(B2:B31)</f>
+        <v>-3.3427958028318887</v>
+      </c>
+      <c r="C33">
+        <f t="shared" ref="C33:E33" si="0">AVERAGE(C2:C31)</f>
+        <v>-4.6041938724218854</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="0"/>
+        <v>-7.2592201756724553</v>
+      </c>
+      <c r="E33">
+        <f t="shared" si="0"/>
+        <v>-9.4859666817193418</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="B34">
+        <f>STDEV(B2:B31)</f>
+        <v>9.1524780411757867</v>
+      </c>
+      <c r="C34">
+        <f t="shared" ref="C34:E34" si="1">STDEV(C2:C31)</f>
+        <v>8.27294939032328</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="1"/>
+        <v>8.6812734913818943</v>
+      </c>
+      <c r="E34">
+        <f t="shared" si="1"/>
+        <v>8.1741337905940483</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>